<commit_message>
Adding the requirements/dependencies file for easy install via pip
</commit_message>
<xml_diff>
--- a/code/Sequencing/Visualize/interactive/example_file.xlsx
+++ b/code/Sequencing/Visualize/interactive/example_file.xlsx
@@ -2475,8 +2475,8 @@
   </sheetPr>
   <dimension ref="A1:U200"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="R1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="T2" activeCellId="0" pane="topLeft" sqref="T2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -2487,11 +2487,12 @@
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="257"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="35.9254901960784"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.0941176470588"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="5.49019607843137"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.0235294117647"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="5.49019607843137"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="11.5764705882353"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -2556,7 +2557,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>21</v>
       </c>
@@ -2621,7 +2622,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>27</v>
       </c>
@@ -2686,7 +2687,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>32</v>
       </c>
@@ -2751,7 +2752,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>36</v>
       </c>
@@ -2816,7 +2817,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>40</v>
       </c>
@@ -2881,7 +2882,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>44</v>
       </c>
@@ -2946,7 +2947,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
         <v>48</v>
       </c>
@@ -3011,7 +3012,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>52</v>
       </c>
@@ -3076,7 +3077,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>56</v>
       </c>
@@ -3141,7 +3142,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>60</v>
       </c>
@@ -3206,7 +3207,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>64</v>
       </c>
@@ -3271,7 +3272,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>68</v>
       </c>
@@ -3336,7 +3337,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>71</v>
       </c>
@@ -3401,7 +3402,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>75</v>
       </c>
@@ -3466,7 +3467,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>79</v>
       </c>
@@ -3531,7 +3532,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>83</v>
       </c>
@@ -3596,7 +3597,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>85</v>
       </c>
@@ -3661,7 +3662,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>89</v>
       </c>
@@ -3726,7 +3727,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>93</v>
       </c>
@@ -3791,7 +3792,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>97</v>
       </c>
@@ -3856,7 +3857,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>101</v>
       </c>
@@ -3921,7 +3922,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>105</v>
       </c>
@@ -3986,7 +3987,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
         <v>110</v>
       </c>
@@ -4051,7 +4052,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
         <v>114</v>
       </c>
@@ -4116,7 +4117,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
         <v>118</v>
       </c>
@@ -4181,7 +4182,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
         <v>122</v>
       </c>
@@ -4246,7 +4247,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>126</v>
       </c>
@@ -4311,7 +4312,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
         <v>130</v>
       </c>
@@ -4376,7 +4377,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
         <v>134</v>
       </c>
@@ -4441,7 +4442,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
         <v>138</v>
       </c>
@@ -4506,7 +4507,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
         <v>142</v>
       </c>
@@ -4571,7 +4572,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
         <v>146</v>
       </c>
@@ -4636,7 +4637,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
         <v>150</v>
       </c>
@@ -4701,7 +4702,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
         <v>154</v>
       </c>
@@ -4766,7 +4767,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
         <v>158</v>
       </c>
@@ -4831,7 +4832,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
         <v>162</v>
       </c>
@@ -4896,7 +4897,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
         <v>166</v>
       </c>
@@ -4961,7 +4962,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
         <v>170</v>
       </c>
@@ -5026,7 +5027,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
         <v>174</v>
       </c>
@@ -5091,7 +5092,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
         <v>178</v>
       </c>
@@ -5156,7 +5157,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
         <v>182</v>
       </c>
@@ -5221,7 +5222,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="43">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
         <v>186</v>
       </c>
@@ -5286,7 +5287,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="44">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
         <v>190</v>
       </c>
@@ -5416,7 +5417,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="46">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
         <v>197</v>
       </c>
@@ -5481,7 +5482,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="47">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
         <v>201</v>
       </c>
@@ -5546,7 +5547,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="48">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
         <v>205</v>
       </c>
@@ -5611,7 +5612,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="49">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
         <v>209</v>
       </c>
@@ -5676,7 +5677,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="50">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="A50" s="0" t="s">
         <v>213</v>
       </c>
@@ -5741,7 +5742,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="51">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="A51" s="0" t="s">
         <v>217</v>
       </c>
@@ -5806,7 +5807,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="52">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="A52" s="0" t="s">
         <v>220</v>
       </c>
@@ -5871,7 +5872,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="53">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="0" t="s">
         <v>224</v>
       </c>
@@ -5936,7 +5937,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="54">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
         <v>228</v>
       </c>
@@ -6001,7 +6002,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="55">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
         <v>232</v>
       </c>
@@ -6066,7 +6067,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="56">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
         <v>236</v>
       </c>
@@ -6131,7 +6132,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="57">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="A57" s="0" t="s">
         <v>240</v>
       </c>
@@ -6196,7 +6197,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="58">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
       <c r="A58" s="0" t="s">
         <v>244</v>
       </c>
@@ -6261,7 +6262,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="59">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="A59" s="0" t="s">
         <v>248</v>
       </c>
@@ -6326,7 +6327,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="60">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="A60" s="0" t="s">
         <v>252</v>
       </c>
@@ -6391,7 +6392,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="61">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
         <v>256</v>
       </c>
@@ -6456,7 +6457,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="62">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
       <c r="A62" s="0" t="s">
         <v>260</v>
       </c>
@@ -6521,7 +6522,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="63">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
       <c r="A63" s="0" t="s">
         <v>264</v>
       </c>
@@ -6586,7 +6587,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="64">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
       <c r="A64" s="0" t="s">
         <v>268</v>
       </c>
@@ -6651,7 +6652,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="65">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
       <c r="A65" s="0" t="s">
         <v>272</v>
       </c>
@@ -6716,7 +6717,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="66">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
       <c r="A66" s="0" t="s">
         <v>276</v>
       </c>
@@ -6781,7 +6782,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="67">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
       <c r="A67" s="0" t="s">
         <v>280</v>
       </c>
@@ -6846,7 +6847,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="68">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="A68" s="0" t="s">
         <v>284</v>
       </c>
@@ -6911,7 +6912,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="69">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
       <c r="A69" s="0" t="s">
         <v>288</v>
       </c>
@@ -6976,7 +6977,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="70">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
       <c r="A70" s="0" t="s">
         <v>292</v>
       </c>
@@ -7041,7 +7042,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="71">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
       <c r="A71" s="0" t="s">
         <v>296</v>
       </c>
@@ -7106,7 +7107,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="72">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
       <c r="A72" s="0" t="s">
         <v>299</v>
       </c>
@@ -7171,7 +7172,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="73">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
       <c r="A73" s="0" t="s">
         <v>303</v>
       </c>
@@ -7236,7 +7237,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="74">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74">
       <c r="A74" s="0" t="s">
         <v>307</v>
       </c>
@@ -7301,7 +7302,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="75">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75">
       <c r="A75" s="0" t="s">
         <v>311</v>
       </c>
@@ -7366,7 +7367,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="76">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
       <c r="A76" s="0" t="s">
         <v>315</v>
       </c>
@@ -7431,7 +7432,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="77">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="77">
       <c r="A77" s="0" t="s">
         <v>319</v>
       </c>
@@ -7496,7 +7497,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="78">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="78">
       <c r="A78" s="0" t="s">
         <v>323</v>
       </c>
@@ -7561,7 +7562,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="79">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="79">
       <c r="A79" s="0" t="s">
         <v>327</v>
       </c>
@@ -7626,7 +7627,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="80">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="80">
       <c r="A80" s="0" t="s">
         <v>331</v>
       </c>
@@ -7691,7 +7692,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="81">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="81">
       <c r="A81" s="0" t="s">
         <v>335</v>
       </c>
@@ -7756,7 +7757,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="82">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="82">
       <c r="A82" s="0" t="s">
         <v>339</v>
       </c>
@@ -7821,7 +7822,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="83">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
       <c r="A83" s="0" t="s">
         <v>343</v>
       </c>
@@ -7886,7 +7887,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="84">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84">
       <c r="A84" s="0" t="s">
         <v>347</v>
       </c>
@@ -7951,7 +7952,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="85">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
       <c r="A85" s="0" t="s">
         <v>351</v>
       </c>
@@ -8016,7 +8017,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="86">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
       <c r="A86" s="0" t="s">
         <v>355</v>
       </c>
@@ -8081,7 +8082,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="87">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
       <c r="A87" s="0" t="s">
         <v>359</v>
       </c>
@@ -8146,7 +8147,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="88">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88">
       <c r="A88" s="0" t="s">
         <v>362</v>
       </c>
@@ -8211,7 +8212,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="89">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
       <c r="A89" s="0" t="s">
         <v>366</v>
       </c>
@@ -8276,7 +8277,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="90">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="90">
       <c r="A90" s="0" t="s">
         <v>369</v>
       </c>
@@ -8406,7 +8407,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="92">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
       <c r="A92" s="0" t="s">
         <v>376</v>
       </c>
@@ -8536,7 +8537,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="94">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
       <c r="A94" s="0" t="s">
         <v>383</v>
       </c>
@@ -8601,7 +8602,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="95">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95">
       <c r="A95" s="0" t="s">
         <v>387</v>
       </c>
@@ -8731,7 +8732,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="97">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="97">
       <c r="A97" s="0" t="s">
         <v>392</v>
       </c>
@@ -8796,7 +8797,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="98">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="98">
       <c r="A98" s="0" t="s">
         <v>395</v>
       </c>
@@ -8861,7 +8862,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="99">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="99">
       <c r="A99" s="0" t="s">
         <v>399</v>
       </c>
@@ -8926,7 +8927,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="100">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
       <c r="A100" s="0" t="s">
         <v>403</v>
       </c>
@@ -8991,7 +8992,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="101">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="101">
       <c r="A101" s="0" t="s">
         <v>406</v>
       </c>
@@ -9056,7 +9057,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="102">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="102">
       <c r="A102" s="0" t="s">
         <v>410</v>
       </c>
@@ -9121,7 +9122,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="103">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="103">
       <c r="A103" s="0" t="s">
         <v>414</v>
       </c>
@@ -9186,7 +9187,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="104">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="104">
       <c r="A104" s="0" t="s">
         <v>417</v>
       </c>
@@ -9251,7 +9252,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="105">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="105">
       <c r="A105" s="0" t="s">
         <v>421</v>
       </c>
@@ -9316,7 +9317,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="106">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="106">
       <c r="A106" s="0" t="s">
         <v>425</v>
       </c>
@@ -9381,7 +9382,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="107">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="107">
       <c r="A107" s="0" t="s">
         <v>429</v>
       </c>
@@ -9446,7 +9447,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="108">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="108">
       <c r="A108" s="0" t="s">
         <v>433</v>
       </c>
@@ -9511,7 +9512,7 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="109">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="109">
       <c r="A109" s="0" t="s">
         <v>437</v>
       </c>
@@ -9576,7 +9577,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="110">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="110">
       <c r="A110" s="0" t="s">
         <v>442</v>
       </c>
@@ -9641,7 +9642,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="111">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="111">
       <c r="A111" s="0" t="s">
         <v>446</v>
       </c>
@@ -9706,7 +9707,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="112">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="112">
       <c r="A112" s="0" t="s">
         <v>450</v>
       </c>
@@ -9771,7 +9772,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="113">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="113">
       <c r="A113" s="0" t="s">
         <v>454</v>
       </c>
@@ -9836,7 +9837,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="114">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="114">
       <c r="A114" s="0" t="s">
         <v>458</v>
       </c>
@@ -9901,7 +9902,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="115">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="115">
       <c r="A115" s="0" t="s">
         <v>462</v>
       </c>
@@ -9966,7 +9967,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="116">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="116">
       <c r="A116" s="0" t="s">
         <v>466</v>
       </c>
@@ -10031,7 +10032,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="117">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="117">
       <c r="A117" s="0" t="s">
         <v>470</v>
       </c>
@@ -10096,7 +10097,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="118">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="118">
       <c r="A118" s="0" t="s">
         <v>474</v>
       </c>
@@ -10161,7 +10162,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="119">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="119">
       <c r="A119" s="0" t="s">
         <v>478</v>
       </c>
@@ -10226,7 +10227,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="120">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="120">
       <c r="A120" s="0" t="s">
         <v>482</v>
       </c>
@@ -10291,7 +10292,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="121">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="121">
       <c r="A121" s="0" t="s">
         <v>486</v>
       </c>
@@ -10356,7 +10357,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="122">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="122">
       <c r="A122" s="0" t="s">
         <v>490</v>
       </c>
@@ -10421,7 +10422,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="123">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="123">
       <c r="A123" s="0" t="s">
         <v>494</v>
       </c>
@@ -10486,7 +10487,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="124">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="124">
       <c r="A124" s="0" t="s">
         <v>498</v>
       </c>
@@ -10551,7 +10552,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="125">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="125">
       <c r="A125" s="0" t="s">
         <v>502</v>
       </c>
@@ -10616,7 +10617,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="126">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="126">
       <c r="A126" s="0" t="s">
         <v>506</v>
       </c>
@@ -10681,7 +10682,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="127">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="127">
       <c r="A127" s="0" t="s">
         <v>509</v>
       </c>
@@ -10746,7 +10747,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="128">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="128">
       <c r="A128" s="0" t="s">
         <v>513</v>
       </c>
@@ -10811,7 +10812,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="129">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="129">
       <c r="A129" s="0" t="s">
         <v>517</v>
       </c>
@@ -10876,7 +10877,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="130">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="130">
       <c r="A130" s="0" t="s">
         <v>521</v>
       </c>
@@ -10941,7 +10942,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="131">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="131">
       <c r="A131" s="0" t="s">
         <v>525</v>
       </c>
@@ -11006,7 +11007,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="132">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="132">
       <c r="A132" s="0" t="s">
         <v>529</v>
       </c>
@@ -11071,7 +11072,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="133">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="133">
       <c r="A133" s="0" t="s">
         <v>533</v>
       </c>
@@ -11136,7 +11137,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="134">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="134">
       <c r="A134" s="0" t="s">
         <v>537</v>
       </c>
@@ -11201,7 +11202,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="135">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="135">
       <c r="A135" s="0" t="s">
         <v>541</v>
       </c>
@@ -11266,7 +11267,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="136">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="136">
       <c r="A136" s="0" t="s">
         <v>545</v>
       </c>
@@ -11331,7 +11332,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="137">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="137">
       <c r="A137" s="0" t="s">
         <v>549</v>
       </c>
@@ -11396,7 +11397,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="138">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="138">
       <c r="A138" s="0" t="s">
         <v>552</v>
       </c>
@@ -11461,7 +11462,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="139">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="139">
       <c r="A139" s="0" t="s">
         <v>556</v>
       </c>
@@ -11526,7 +11527,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="140">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="140">
       <c r="A140" s="0" t="s">
         <v>559</v>
       </c>
@@ -11591,7 +11592,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="141">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="141">
       <c r="A141" s="0" t="s">
         <v>563</v>
       </c>
@@ -11656,7 +11657,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="142">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="142">
       <c r="A142" s="0" t="s">
         <v>567</v>
       </c>
@@ -11721,7 +11722,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="143">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="143">
       <c r="A143" s="0" t="s">
         <v>571</v>
       </c>
@@ -11786,7 +11787,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="144">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="144">
       <c r="A144" s="0" t="s">
         <v>575</v>
       </c>
@@ -11851,7 +11852,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="145">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="145">
       <c r="A145" s="0" t="s">
         <v>579</v>
       </c>
@@ -11916,7 +11917,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="146">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="146">
       <c r="A146" s="0" t="s">
         <v>582</v>
       </c>
@@ -12046,7 +12047,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="148">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="148">
       <c r="A148" s="0" t="s">
         <v>587</v>
       </c>
@@ -12176,7 +12177,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="150">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="150">
       <c r="A150" s="0" t="s">
         <v>592</v>
       </c>
@@ -12241,7 +12242,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="151">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="151">
       <c r="A151" s="0" t="s">
         <v>596</v>
       </c>
@@ -12306,7 +12307,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="152">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="152">
       <c r="A152" s="0" t="s">
         <v>600</v>
       </c>
@@ -12371,7 +12372,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="153">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="153">
       <c r="A153" s="0" t="s">
         <v>604</v>
       </c>
@@ -12436,7 +12437,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="154">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="154">
       <c r="A154" s="0" t="s">
         <v>608</v>
       </c>
@@ -12501,7 +12502,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="155">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="155">
       <c r="A155" s="0" t="s">
         <v>612</v>
       </c>
@@ -12566,7 +12567,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="156">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="156">
       <c r="A156" s="0" t="s">
         <v>616</v>
       </c>
@@ -12631,7 +12632,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="157">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="157">
       <c r="A157" s="0" t="s">
         <v>619</v>
       </c>
@@ -12696,7 +12697,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="158">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="158">
       <c r="A158" s="0" t="s">
         <v>623</v>
       </c>
@@ -12761,7 +12762,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="159">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="159">
       <c r="A159" s="0" t="s">
         <v>627</v>
       </c>
@@ -12826,7 +12827,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="160">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="160">
       <c r="A160" s="0" t="s">
         <v>631</v>
       </c>
@@ -12891,7 +12892,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="161">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="161">
       <c r="A161" s="0" t="s">
         <v>634</v>
       </c>
@@ -12956,7 +12957,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="162">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="162">
       <c r="A162" s="0" t="s">
         <v>638</v>
       </c>
@@ -13021,7 +13022,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="163">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="163">
       <c r="A163" s="0" t="s">
         <v>642</v>
       </c>
@@ -13086,7 +13087,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="164">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="164">
       <c r="A164" s="0" t="s">
         <v>646</v>
       </c>
@@ -13151,7 +13152,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="165">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="165">
       <c r="A165" s="0" t="s">
         <v>650</v>
       </c>
@@ -13216,7 +13217,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="166">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="166">
       <c r="A166" s="0" t="s">
         <v>654</v>
       </c>
@@ -13281,7 +13282,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="167">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="167">
       <c r="A167" s="0" t="s">
         <v>658</v>
       </c>
@@ -13346,7 +13347,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="168">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="168">
       <c r="A168" s="0" t="s">
         <v>662</v>
       </c>
@@ -13411,7 +13412,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="169">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="169">
       <c r="A169" s="0" t="s">
         <v>666</v>
       </c>
@@ -13476,7 +13477,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="170">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="170">
       <c r="A170" s="0" t="s">
         <v>670</v>
       </c>
@@ -13541,7 +13542,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="171">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="171">
       <c r="A171" s="0" t="s">
         <v>674</v>
       </c>
@@ -13606,7 +13607,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="172">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="172">
       <c r="A172" s="0" t="s">
         <v>678</v>
       </c>
@@ -13671,7 +13672,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="173">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="173">
       <c r="A173" s="0" t="s">
         <v>682</v>
       </c>
@@ -13801,7 +13802,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="175">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="175">
       <c r="A175" s="0" t="s">
         <v>687</v>
       </c>
@@ -13866,7 +13867,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="176">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="176">
       <c r="A176" s="0" t="s">
         <v>690</v>
       </c>
@@ -13931,7 +13932,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="177">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="177">
       <c r="A177" s="0" t="s">
         <v>694</v>
       </c>
@@ -13996,7 +13997,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="178">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="178">
       <c r="A178" s="0" t="s">
         <v>698</v>
       </c>
@@ -14061,7 +14062,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="179">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="179">
       <c r="A179" s="0" t="s">
         <v>702</v>
       </c>
@@ -14126,7 +14127,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="180">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="180">
       <c r="A180" s="0" t="s">
         <v>706</v>
       </c>
@@ -14191,7 +14192,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="181">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="181">
       <c r="A181" s="0" t="s">
         <v>710</v>
       </c>
@@ -14256,7 +14257,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="182">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="182">
       <c r="A182" s="0" t="s">
         <v>714</v>
       </c>
@@ -14321,7 +14322,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="183">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="183">
       <c r="A183" s="0" t="s">
         <v>718</v>
       </c>
@@ -14386,7 +14387,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="184">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="184">
       <c r="A184" s="0" t="s">
         <v>722</v>
       </c>
@@ -14451,7 +14452,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="185">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="185">
       <c r="A185" s="0" t="s">
         <v>726</v>
       </c>
@@ -14516,7 +14517,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="186">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="186">
       <c r="A186" s="0" t="s">
         <v>730</v>
       </c>
@@ -14581,7 +14582,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="187">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="187">
       <c r="A187" s="0" t="s">
         <v>734</v>
       </c>
@@ -14646,7 +14647,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="188">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="188">
       <c r="A188" s="0" t="s">
         <v>738</v>
       </c>
@@ -14711,7 +14712,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="189">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="189">
       <c r="A189" s="0" t="s">
         <v>742</v>
       </c>
@@ -14776,7 +14777,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="190">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="190">
       <c r="A190" s="0" t="s">
         <v>746</v>
       </c>
@@ -14841,7 +14842,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="191">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="191">
       <c r="A191" s="0" t="s">
         <v>749</v>
       </c>
@@ -14906,7 +14907,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="192">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="192">
       <c r="A192" s="0" t="s">
         <v>753</v>
       </c>
@@ -14971,7 +14972,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="193">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="193">
       <c r="A193" s="0" t="s">
         <v>757</v>
       </c>
@@ -15036,7 +15037,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="194">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="194">
       <c r="A194" s="0" t="s">
         <v>761</v>
       </c>
@@ -15101,7 +15102,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="195">
       <c r="A195" s="0" t="s">
         <v>764</v>
       </c>
@@ -15166,7 +15167,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="196">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="196">
       <c r="A196" s="0" t="s">
         <v>768</v>
       </c>
@@ -15231,7 +15232,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="197">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="197">
       <c r="A197" s="0" t="s">
         <v>772</v>
       </c>
@@ -15296,7 +15297,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="198">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="198">
       <c r="A198" s="0" t="s">
         <v>776</v>
       </c>
@@ -15361,7 +15362,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="199">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="199">
       <c r="A199" s="0" t="s">
         <v>780</v>
       </c>
@@ -15426,7 +15427,7 @@
         <v>441</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="200">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="200">
       <c r="A200" s="0" t="s">
         <v>784</v>
       </c>

</xml_diff>